<commit_message>
added phe_quantile example code and moved code to assign highergeog to grouping set outside of if statement.  Updated phe_quantile documentation.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Rate.xlsx
+++ b/tests/testthat/testdata_Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA1458C-8178-4E91-A6C0-7F8DC31CCA4E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F2EC38-0182-4CFB-8AD4-0336BB2B1BC0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Rate" sheetId="2" r:id="rId1"/>
@@ -451,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -1682,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD39EBE6-76F1-4DEA-ABB6-5CC513AA3B0B}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,93 +1755,59 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
+      <c r="A3" t="s">
+        <v>25</v>
       </c>
       <c r="B3">
-        <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A3,testdata_Rate!B$2:B$33)</f>
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A3,testdata_Rate!C$2:C$33)</f>
-        <v>400</v>
-      </c>
-      <c r="D3">
-        <v>5000</v>
-      </c>
-      <c r="E3">
-        <v>3052.8572087189841</v>
-      </c>
-      <c r="F3">
-        <v>7722.4700922992661</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="4">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3">
         <v>100000</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A4,testdata_Rate!B$2:B$33)</f>
-        <v>80</v>
-      </c>
-      <c r="C4">
-        <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A4,testdata_Rate!C$2:C$33)</f>
-        <v>400</v>
-      </c>
-      <c r="D4">
-        <v>20000</v>
-      </c>
-      <c r="E4">
-        <v>15858.21780470269</v>
-      </c>
-      <c r="F4">
-        <v>24892.038099730591</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4">
         <v>100000</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A5,testdata_Rate!B$2:B$33)</f>
-        <v>260</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A5,testdata_Rate!C$2:C$33)</f>
         <v>400</v>
       </c>
       <c r="D5">
-        <v>65000</v>
+        <v>5000</v>
       </c>
       <c r="E5">
-        <v>57338.247579389856</v>
+        <v>3052.8572087189841</v>
       </c>
       <c r="F5">
-        <v>73400.310929637635</v>
+        <v>7722.4700922992661</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>11</v>
@@ -1858,24 +1824,24 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A6,testdata_Rate!B$2:B$33)</f>
-        <v>39424</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A6,testdata_Rate!C$2:C$33)</f>
-        <v>49380</v>
+        <v>400</v>
       </c>
       <c r="D6">
-        <v>79837.991089509916</v>
+        <v>20000</v>
       </c>
       <c r="E6">
-        <v>79051.81799297237</v>
+        <v>15858.21780470269</v>
       </c>
       <c r="F6">
-        <v>80630.035462060783</v>
+        <v>24892.038099730591</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>11</v>
@@ -1892,24 +1858,24 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A7,testdata_Rate!B$2:B$33)</f>
-        <v>31105824</v>
+        <v>260</v>
       </c>
       <c r="C7">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A7,testdata_Rate!C$2:C$33)</f>
-        <v>30257346708</v>
+        <v>400</v>
       </c>
       <c r="D7">
-        <v>102.80420256339154</v>
+        <v>65000</v>
       </c>
       <c r="E7">
-        <v>102.76807817760378</v>
+        <v>57338.247579389856</v>
       </c>
       <c r="F7">
-        <v>102.84033651539011</v>
+        <v>73400.310929637635</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>11</v>
@@ -1926,24 +1892,24 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A8,testdata_Rate!B$2:B$33)</f>
-        <v>888</v>
+        <v>39424</v>
       </c>
       <c r="C8">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A8,testdata_Rate!C$2:C$33)</f>
-        <v>12860</v>
+        <v>49380</v>
       </c>
       <c r="D8">
-        <v>6905.1321928460338</v>
+        <v>79837.991089509916</v>
       </c>
       <c r="E8">
-        <v>6458.3723204675634</v>
+        <v>79051.81799297237</v>
       </c>
       <c r="F8">
-        <v>7374.6521642203033</v>
+        <v>80630.035462060783</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>11</v>
@@ -1960,78 +1926,112 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A9,testdata_Rate!B$2:B$33)</f>
-        <v>3996</v>
+        <v>31105824</v>
       </c>
       <c r="C9">
         <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A9,testdata_Rate!C$2:C$33)</f>
+        <v>30257346708</v>
+      </c>
+      <c r="D9">
+        <v>102.80420256339154</v>
+      </c>
+      <c r="E9">
+        <v>102.76807817760378</v>
+      </c>
+      <c r="F9">
+        <v>102.84033651539011</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A10,testdata_Rate!B$2:B$33)</f>
+        <v>888</v>
+      </c>
+      <c r="C10">
+        <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A10,testdata_Rate!C$2:C$33)</f>
+        <v>12860</v>
+      </c>
+      <c r="D10">
+        <v>6905.1321928460338</v>
+      </c>
+      <c r="E10">
+        <v>6458.3723204675634</v>
+      </c>
+      <c r="F10">
+        <v>7374.6521642203033</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A11,testdata_Rate!B$2:B$33)</f>
+        <v>3996</v>
+      </c>
+      <c r="C11">
+        <f>SUMIF(testdata_Rate!$A$2:$A$33,testdata_Rate_g!$A11,testdata_Rate!C$2:C$33)</f>
         <v>13824</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>28906.25</v>
       </c>
-      <c r="E9">
+      <c r="E11">
         <v>28016.873508380959</v>
       </c>
-      <c r="F9">
+      <c r="F11">
         <v>29816.675067891891</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="4">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11">
+      <c r="G11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="4">
         <v>100000</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>

</xml_diff>